<commit_message>
CMM018M: add template report
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/マスタリストのEXCEL出力.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/マスタリストのEXCEL出力.xlsx
@@ -44818,7 +44818,7 @@
   <pageSetup paperSize="9" scale="68" orientation="portrait" useFirstPageNumber="1" errors="NA" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;9【会社】日通システム株式会社&amp;C&amp;"ＭＳ ゴシック,Bold"&amp;16会社の承認ルート&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;9&amp;D&amp;T
-&amp;Nページ</oddHeader>
+&amp;Pページ</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
@@ -44827,8 +44827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12"/>
@@ -44932,7 +44932,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageLayout" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12"/>
@@ -45025,7 +45025,7 @@
   <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;9【会社】日通システム株式会社&amp;C&amp;"ＭＳ ゴシック,Bold"&amp;16個人の承認ルート&amp;R&amp;"ＭＳ ゴシック,Regular"&amp;9&amp;D&amp;T
-&amp;Nページ</oddHeader>
+&amp;Pページ</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CMM018 - M: print sheet Company
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/マスタリストのEXCEL出力.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/マスタリストのEXCEL出力.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="770"/>
   </bookViews>
   <sheets>
-    <sheet name="会社別" sheetId="36" r:id="rId1"/>
-    <sheet name="職場別" sheetId="39" r:id="rId2"/>
+    <sheet name="会社別" sheetId="43" r:id="rId1"/>
+    <sheet name="職場別" sheetId="42" r:id="rId2"/>
     <sheet name="個人別" sheetId="40" r:id="rId3"/>
   </sheets>
   <externalReferences>
@@ -98,6 +98,10 @@
     <definedName name="CULC.cal_index_size" localSheetId="2">[3]!CULC.cal_index_size</definedName>
     <definedName name="CULC.cal_index_size" localSheetId="1">[3]!CULC.cal_index_size</definedName>
     <definedName name="CULC.cal_index_size">[3]!CULC.cal_index_size</definedName>
+    <definedName name="C保守単価" localSheetId="0">'[4]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守単価" localSheetId="2">'[4]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守単価" localSheetId="1">'[4]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守委託単価" localSheetId="0">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守委託単価" localSheetId="2">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守委託単価" localSheetId="1">'[4]見積明細(ハードのみ）'!#REF!</definedName>
@@ -106,10 +110,6 @@
     <definedName name="C保守支援単価" localSheetId="2">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守支援単価" localSheetId="1">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守支援単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守単価" localSheetId="0">'[4]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守単価" localSheetId="2">'[4]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守単価" localSheetId="1">'[4]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="DDDD" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="def" localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="def" localSheetId="2" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
@@ -143,6 +143,8 @@
     <definedName name="ＬＨ" localSheetId="2">#REF!</definedName>
     <definedName name="ＬＨ" localSheetId="1">#REF!</definedName>
     <definedName name="ＬＨ">#REF!</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="ＬサＨ" localSheetId="0">#REF!</definedName>
     <definedName name="ＬサＨ" localSheetId="2">#REF!</definedName>
@@ -200,10 +202,10 @@
     <definedName name="PG田中" localSheetId="2">#REF!</definedName>
     <definedName name="PG田中" localSheetId="1">#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">会社別!$A$1:$N$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">会社別!$A$1:$N$68</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">個人別!$A$1:$N$68</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">職場別!$A$1:$N$68</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">会社別!$1:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">会社別!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">個人別!$1:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">職場別!$1:$3</definedName>
     <definedName name="PrintDaicho" localSheetId="0">[9]!PrintDaicho</definedName>
@@ -359,14 +361,90 @@
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ" localSheetId="2">#REF!</definedName>
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ" localSheetId="1">#REF!</definedName>
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ">#REF!</definedName>
+    <definedName name="人日原価" localSheetId="0">#REF!</definedName>
+    <definedName name="人日原価" localSheetId="2">#REF!</definedName>
+    <definedName name="人日原価" localSheetId="1">#REF!</definedName>
+    <definedName name="人日原価">#REF!</definedName>
+    <definedName name="仕切り">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="仕切単価">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="住民税115" localSheetId="0">#REF!</definedName>
+    <definedName name="住民税115" localSheetId="2">#REF!</definedName>
+    <definedName name="住民税115" localSheetId="1">#REF!</definedName>
+    <definedName name="住民税115">#REF!</definedName>
+    <definedName name="住民税96" localSheetId="0">#REF!</definedName>
+    <definedName name="住民税96" localSheetId="2">#REF!</definedName>
+    <definedName name="住民税96" localSheetId="1">#REF!</definedName>
+    <definedName name="住民税96">#REF!</definedName>
+    <definedName name="住民税納付先の登録7" localSheetId="0">#REF!</definedName>
+    <definedName name="住民税納付先の登録7" localSheetId="2">#REF!</definedName>
+    <definedName name="住民税納付先の登録7" localSheetId="1">#REF!</definedName>
+    <definedName name="住民税納付先の登録7">#REF!</definedName>
+    <definedName name="価格表" localSheetId="0">#REF!</definedName>
+    <definedName name="価格表" localSheetId="2">#REF!</definedName>
+    <definedName name="価格表" localSheetId="1">#REF!</definedName>
+    <definedName name="価格表">#REF!</definedName>
+    <definedName name="保守単価">'[4]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
+    <definedName name="保守委託単価">'[4]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
+    <definedName name="保守支援単価">'[4]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
+    <definedName name="値引単価">'[4]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
+    <definedName name="備考">'[4]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
+    <definedName name="単価" localSheetId="0">#REF!</definedName>
+    <definedName name="単価" localSheetId="2">#REF!</definedName>
+    <definedName name="単価" localSheetId="1">#REF!</definedName>
+    <definedName name="単価">#REF!</definedName>
+    <definedName name="単価種別" localSheetId="0">#REF!</definedName>
+    <definedName name="単価種別" localSheetId="2">#REF!</definedName>
+    <definedName name="単価種別" localSheetId="1">#REF!</definedName>
+    <definedName name="単価種別">#REF!</definedName>
     <definedName name="印刷" localSheetId="0">[14]!印刷</definedName>
     <definedName name="印刷" localSheetId="2">[14]!印刷</definedName>
     <definedName name="印刷" localSheetId="1">[14]!印刷</definedName>
     <definedName name="印刷">[14]!印刷</definedName>
-    <definedName name="価格表" localSheetId="0">#REF!</definedName>
-    <definedName name="価格表" localSheetId="2">#REF!</definedName>
-    <definedName name="価格表" localSheetId="1">#REF!</definedName>
-    <definedName name="価格表">#REF!</definedName>
+    <definedName name="原価" localSheetId="0">#REF!</definedName>
+    <definedName name="原価" localSheetId="2">#REF!</definedName>
+    <definedName name="原価" localSheetId="1">#REF!</definedName>
+    <definedName name="原価">#REF!</definedName>
+    <definedName name="売値" localSheetId="0">#REF!</definedName>
+    <definedName name="売値" localSheetId="2">#REF!</definedName>
+    <definedName name="売値" localSheetId="1">#REF!</definedName>
+    <definedName name="売値">#REF!</definedName>
+    <definedName name="定価" localSheetId="0">#REF!</definedName>
+    <definedName name="定価" localSheetId="2">#REF!</definedName>
+    <definedName name="定価" localSheetId="1">#REF!</definedName>
+    <definedName name="定価">#REF!</definedName>
+    <definedName name="宿泊" localSheetId="0">#REF!</definedName>
+    <definedName name="宿泊" localSheetId="2">#REF!</definedName>
+    <definedName name="宿泊" localSheetId="1">#REF!</definedName>
+    <definedName name="宿泊">#REF!</definedName>
+    <definedName name="宿泊単金" localSheetId="0">#REF!</definedName>
+    <definedName name="宿泊単金" localSheetId="2">#REF!</definedName>
+    <definedName name="宿泊単金" localSheetId="1">#REF!</definedName>
+    <definedName name="宿泊単金">#REF!</definedName>
+    <definedName name="工程別生産性" localSheetId="0">#REF!</definedName>
+    <definedName name="工程別生産性" localSheetId="2">#REF!</definedName>
+    <definedName name="工程別生産性" localSheetId="1">#REF!</definedName>
+    <definedName name="工程別生産性">#REF!</definedName>
+    <definedName name="日帰り" localSheetId="0">#REF!</definedName>
+    <definedName name="日帰り" localSheetId="2">#REF!</definedName>
+    <definedName name="日帰り" localSheetId="1">#REF!</definedName>
+    <definedName name="日帰り">#REF!</definedName>
+    <definedName name="日帰り単金" localSheetId="0">#REF!</definedName>
+    <definedName name="日帰り単金" localSheetId="2">#REF!</definedName>
+    <definedName name="日帰り単金" localSheetId="1">#REF!</definedName>
+    <definedName name="日帰り単金">#REF!</definedName>
+    <definedName name="概要_基準日設定" localSheetId="0" hidden="1">#REF!</definedName>
+    <definedName name="概要_基準日設定" localSheetId="2" hidden="1">#REF!</definedName>
+    <definedName name="概要_基準日設定" localSheetId="1" hidden="1">#REF!</definedName>
+    <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
+    <definedName name="標準価格">'[4]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
+    <definedName name="機種SORT" localSheetId="0">[15]!機種SORT</definedName>
+    <definedName name="機種SORT" localSheetId="2">[15]!機種SORT</definedName>
+    <definedName name="機種SORT" localSheetId="1">[15]!機種SORT</definedName>
+    <definedName name="機種SORT">[16]!機種SORT</definedName>
+    <definedName name="機能別原価" localSheetId="0">#REF!</definedName>
+    <definedName name="機能別原価" localSheetId="2">#REF!</definedName>
+    <definedName name="機能別原価" localSheetId="1">#REF!</definedName>
+    <definedName name="機能別原価">#REF!</definedName>
     <definedName name="画面1" localSheetId="0">#REF!</definedName>
     <definedName name="画面1" localSheetId="2">#REF!</definedName>
     <definedName name="画面1" localSheetId="1">#REF!</definedName>
@@ -395,23 +473,31 @@
     <definedName name="画面7" localSheetId="2">#REF!</definedName>
     <definedName name="画面7" localSheetId="1">#REF!</definedName>
     <definedName name="画面7">#REF!</definedName>
+    <definedName name="直扱単価">'[4]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
+    <definedName name="社共単価">'[4]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
+    <definedName name="種別" localSheetId="0">#REF!</definedName>
+    <definedName name="種別" localSheetId="2">#REF!</definedName>
+    <definedName name="種別" localSheetId="1">#REF!</definedName>
+    <definedName name="種別">#REF!</definedName>
+    <definedName name="終了" localSheetId="0">[17]!終了</definedName>
+    <definedName name="終了" localSheetId="2">[17]!終了</definedName>
+    <definedName name="終了" localSheetId="1">[17]!終了</definedName>
+    <definedName name="終了">[17]!終了</definedName>
+    <definedName name="見やすく" localSheetId="0">[13]!見やすく</definedName>
+    <definedName name="見やすく" localSheetId="2">[13]!見やすく</definedName>
+    <definedName name="見やすく" localSheetId="1">[13]!見やすく</definedName>
+    <definedName name="見やすく">[13]!見やすく</definedName>
+    <definedName name="見積工数" localSheetId="0">#REF!</definedName>
+    <definedName name="見積工数" localSheetId="2">#REF!</definedName>
+    <definedName name="見積工数" localSheetId="1">#REF!</definedName>
+    <definedName name="見積工数">#REF!</definedName>
     <definedName name="解析">#N/A</definedName>
-    <definedName name="概要_基準日設定" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="概要_基準日設定" localSheetId="2" hidden="1">#REF!</definedName>
-    <definedName name="概要_基準日設定" localSheetId="1" hidden="1">#REF!</definedName>
-    <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
-    <definedName name="関連表" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="関連表" localSheetId="2" hidden="1">#REF!</definedName>
-    <definedName name="関連表" localSheetId="1" hidden="1">#REF!</definedName>
-    <definedName name="関連表" hidden="1">#REF!</definedName>
-    <definedName name="機種SORT" localSheetId="0">[15]!機種SORT</definedName>
-    <definedName name="機種SORT" localSheetId="2">[15]!機種SORT</definedName>
-    <definedName name="機種SORT" localSheetId="1">[15]!機種SORT</definedName>
-    <definedName name="機種SORT">[16]!機種SORT</definedName>
-    <definedName name="機能別原価" localSheetId="0">#REF!</definedName>
-    <definedName name="機能別原価" localSheetId="2">#REF!</definedName>
-    <definedName name="機能別原価" localSheetId="1">#REF!</definedName>
-    <definedName name="機能別原価">#REF!</definedName>
+    <definedName name="設計書">#N/A</definedName>
+    <definedName name="部">'[4]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
+    <definedName name="部門別時間外労働手当状況" localSheetId="0">#REF!</definedName>
+    <definedName name="部門別時間外労働手当状況" localSheetId="2">#REF!</definedName>
+    <definedName name="部門別時間外労働手当状況" localSheetId="1">#REF!</definedName>
+    <definedName name="部門別時間外労働手当状況">#REF!</definedName>
     <definedName name="銀行の登録48" localSheetId="0">#REF!</definedName>
     <definedName name="銀行の登録48" localSheetId="2">#REF!</definedName>
     <definedName name="銀行の登録48" localSheetId="1">#REF!</definedName>
@@ -424,22 +510,14 @@
     <definedName name="銀行の登録7" localSheetId="2">#REF!</definedName>
     <definedName name="銀行の登録7" localSheetId="1">#REF!</definedName>
     <definedName name="銀行の登録7">#REF!</definedName>
-    <definedName name="見やすく" localSheetId="0">[13]!見やすく</definedName>
-    <definedName name="見やすく" localSheetId="2">[13]!見やすく</definedName>
-    <definedName name="見やすく" localSheetId="1">[13]!見やすく</definedName>
-    <definedName name="見やすく">[13]!見やすく</definedName>
-    <definedName name="見積工数" localSheetId="0">#REF!</definedName>
-    <definedName name="見積工数" localSheetId="2">#REF!</definedName>
-    <definedName name="見積工数" localSheetId="1">#REF!</definedName>
-    <definedName name="見積工数">#REF!</definedName>
-    <definedName name="原価" localSheetId="0">#REF!</definedName>
-    <definedName name="原価" localSheetId="2">#REF!</definedName>
-    <definedName name="原価" localSheetId="1">#REF!</definedName>
-    <definedName name="原価">#REF!</definedName>
-    <definedName name="工程別生産性" localSheetId="0">#REF!</definedName>
-    <definedName name="工程別生産性" localSheetId="2">#REF!</definedName>
-    <definedName name="工程別生産性" localSheetId="1">#REF!</definedName>
-    <definedName name="工程別生産性">#REF!</definedName>
+    <definedName name="関連表" localSheetId="0" hidden="1">#REF!</definedName>
+    <definedName name="関連表" localSheetId="2" hidden="1">#REF!</definedName>
+    <definedName name="関連表" localSheetId="1" hidden="1">#REF!</definedName>
+    <definedName name="関連表" hidden="1">#REF!</definedName>
+    <definedName name="電車" localSheetId="0">#REF!</definedName>
+    <definedName name="電車" localSheetId="2">#REF!</definedName>
+    <definedName name="電車" localSheetId="1">#REF!</definedName>
+    <definedName name="電車">#REF!</definedName>
     <definedName name="項目名の登録1" localSheetId="0">#REF!</definedName>
     <definedName name="項目名の登録1" localSheetId="2">#REF!</definedName>
     <definedName name="項目名の登録1" localSheetId="1">#REF!</definedName>
@@ -472,93 +550,17 @@
     <definedName name="項目名の登録8" localSheetId="2">#REF!</definedName>
     <definedName name="項目名の登録8" localSheetId="1">#REF!</definedName>
     <definedName name="項目名の登録8">#REF!</definedName>
-    <definedName name="仕切り">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
-    <definedName name="仕切単価">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
-    <definedName name="社共単価">'[4]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
-    <definedName name="種別" localSheetId="0">#REF!</definedName>
-    <definedName name="種別" localSheetId="2">#REF!</definedName>
-    <definedName name="種別" localSheetId="1">#REF!</definedName>
-    <definedName name="種別">#REF!</definedName>
-    <definedName name="終了" localSheetId="0">[17]!終了</definedName>
-    <definedName name="終了" localSheetId="2">[17]!終了</definedName>
-    <definedName name="終了" localSheetId="1">[17]!終了</definedName>
-    <definedName name="終了">[17]!終了</definedName>
-    <definedName name="住民税115" localSheetId="0">#REF!</definedName>
-    <definedName name="住民税115" localSheetId="2">#REF!</definedName>
-    <definedName name="住民税115" localSheetId="1">#REF!</definedName>
-    <definedName name="住民税115">#REF!</definedName>
-    <definedName name="住民税96" localSheetId="0">#REF!</definedName>
-    <definedName name="住民税96" localSheetId="2">#REF!</definedName>
-    <definedName name="住民税96" localSheetId="1">#REF!</definedName>
-    <definedName name="住民税96">#REF!</definedName>
-    <definedName name="住民税納付先の登録7" localSheetId="0">#REF!</definedName>
-    <definedName name="住民税納付先の登録7" localSheetId="2">#REF!</definedName>
-    <definedName name="住民税納付先の登録7" localSheetId="1">#REF!</definedName>
-    <definedName name="住民税納付先の登録7">#REF!</definedName>
-    <definedName name="宿泊" localSheetId="0">#REF!</definedName>
-    <definedName name="宿泊" localSheetId="2">#REF!</definedName>
-    <definedName name="宿泊" localSheetId="1">#REF!</definedName>
-    <definedName name="宿泊">#REF!</definedName>
-    <definedName name="宿泊単金" localSheetId="0">#REF!</definedName>
-    <definedName name="宿泊単金" localSheetId="2">#REF!</definedName>
-    <definedName name="宿泊単金" localSheetId="1">#REF!</definedName>
-    <definedName name="宿泊単金">#REF!</definedName>
-    <definedName name="人日原価" localSheetId="0">#REF!</definedName>
-    <definedName name="人日原価" localSheetId="2">#REF!</definedName>
-    <definedName name="人日原価" localSheetId="1">#REF!</definedName>
-    <definedName name="人日原価">#REF!</definedName>
-    <definedName name="設計書">#N/A</definedName>
-    <definedName name="単価" localSheetId="0">#REF!</definedName>
-    <definedName name="単価" localSheetId="2">#REF!</definedName>
-    <definedName name="単価" localSheetId="1">#REF!</definedName>
-    <definedName name="単価">#REF!</definedName>
-    <definedName name="単価種別" localSheetId="0">#REF!</definedName>
-    <definedName name="単価種別" localSheetId="2">#REF!</definedName>
-    <definedName name="単価種別" localSheetId="1">#REF!</definedName>
-    <definedName name="単価種別">#REF!</definedName>
-    <definedName name="値引単価">'[4]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
-    <definedName name="直扱単価">'[4]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
-    <definedName name="定価" localSheetId="0">#REF!</definedName>
-    <definedName name="定価" localSheetId="2">#REF!</definedName>
-    <definedName name="定価" localSheetId="1">#REF!</definedName>
-    <definedName name="定価">#REF!</definedName>
-    <definedName name="電車" localSheetId="0">#REF!</definedName>
-    <definedName name="電車" localSheetId="2">#REF!</definedName>
-    <definedName name="電車" localSheetId="1">#REF!</definedName>
-    <definedName name="電車">#REF!</definedName>
-    <definedName name="日帰り" localSheetId="0">#REF!</definedName>
-    <definedName name="日帰り" localSheetId="2">#REF!</definedName>
-    <definedName name="日帰り" localSheetId="1">#REF!</definedName>
-    <definedName name="日帰り">#REF!</definedName>
-    <definedName name="日帰り単金" localSheetId="0">#REF!</definedName>
-    <definedName name="日帰り単金" localSheetId="2">#REF!</definedName>
-    <definedName name="日帰り単金" localSheetId="1">#REF!</definedName>
-    <definedName name="日帰り単金">#REF!</definedName>
-    <definedName name="売値" localSheetId="0">#REF!</definedName>
-    <definedName name="売値" localSheetId="2">#REF!</definedName>
-    <definedName name="売値" localSheetId="1">#REF!</definedName>
-    <definedName name="売値">#REF!</definedName>
     <definedName name="飛行機" localSheetId="0">#REF!</definedName>
     <definedName name="飛行機" localSheetId="2">#REF!</definedName>
     <definedName name="飛行機" localSheetId="1">#REF!</definedName>
     <definedName name="飛行機">#REF!</definedName>
-    <definedName name="備考">'[4]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
-    <definedName name="標準価格">'[4]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
-    <definedName name="部">'[4]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
-    <definedName name="部門別時間外労働手当状況" localSheetId="0">#REF!</definedName>
-    <definedName name="部門別時間外労働手当状況" localSheetId="2">#REF!</definedName>
-    <definedName name="部門別時間外労働手当状況" localSheetId="1">#REF!</definedName>
-    <definedName name="部門別時間外労働手当状況">#REF!</definedName>
-    <definedName name="保守委託単価">'[4]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
-    <definedName name="保守支援単価">'[4]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
-    <definedName name="保守単価">'[4]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>期間</t>
     <rPh sb="0" eb="2">
@@ -572,10 +574,6 @@
   </si>
   <si>
     <t>フェーズ3⇒</t>
-  </si>
-  <si>
-    <t>フェーズ2⇒</t>
-    <phoneticPr fontId="11"/>
   </si>
   <si>
     <t>フェーズ4⇒</t>
@@ -607,14 +605,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -622,7 +620,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -630,7 +628,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -643,7 +641,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -671,7 +669,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -800,7 +798,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3">
       <alignment vertical="center"/>
@@ -814,9 +812,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -824,6 +819,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -44752,131 +44753,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="B1" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="55" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="1.625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="2.75" style="1"/>
-    <col min="16" max="16" width="1.125" style="1" customWidth="1"/>
-    <col min="17" max="37" width="2.75" style="1" hidden="1" customWidth="1"/>
-    <col min="38" max="16384" width="2.75" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" thickBot="1">
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-  </mergeCells>
-  <phoneticPr fontId="5"/>
-  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.59055118110236204" bottom="0.59055118110236204" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="68" orientation="portrait" useFirstPageNumber="1" errors="NA" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"ＭＳ ゴシック,太字"&amp;16会社の承認ルート&amp;R&amp;"ＭＳ ゴシック,標準"&amp;9&amp;D &amp;T
-&amp;Pページ</oddHeader>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
-  <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="12"/>
-  <cols>
-    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="1.625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="2.75" style="1"/>
+    <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="1.5703125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="2.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1">
@@ -44909,30 +44808,30 @@
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7" t="s">
-        <v>4</v>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>3</v>
       </c>
-      <c r="K3" s="7"/>
+      <c r="K3" s="9"/>
       <c r="L3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="2"/>
@@ -44945,42 +44844,40 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
   </mergeCells>
-  <phoneticPr fontId="5"/>
-  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.59055118110236204" bottom="0.59055118110236204" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="65" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"ＭＳ ゴシック,太字"&amp;16職場の承認ルート&amp;R&amp;"ＭＳ ゴシック,標準"&amp;9&amp;D &amp;T
+    <oddHeader>&amp;C&amp;"ＭＳ ゴシック,太字"&amp;16会社の承認ルート&amp;R&amp;"ＭＳ ゴシック,標準"&amp;9&amp;D &amp;T
 &amp;Pページ</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="1.625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="2.75" style="1"/>
+    <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="1.5703125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="2.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1">
@@ -45013,30 +44910,132 @@
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.59055118110236204" bottom="0.59055118110236204" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"ＭＳ ゴシック,太字"&amp;16職場の承認ルート&amp;R&amp;"ＭＳ ゴシック,標準"&amp;9&amp;D &amp;T
+&amp;Pページ</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="55" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="1.5703125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="2.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15" customHeight="1">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" customHeight="1" thickBot="1">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E3" s="8"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7" t="s">
-        <v>4</v>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>3</v>
       </c>
-      <c r="K3" s="7"/>
+      <c r="K3" s="9"/>
       <c r="L3" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="2"/>

</xml_diff>

<commit_message>
CMM018_2次: M, templace thay đổi
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/マスタリストのEXCEL出力.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/マスタリストのEXCEL出力.xlsx
@@ -98,10 +98,6 @@
     <definedName name="CULC.cal_index_size" localSheetId="2">[3]!CULC.cal_index_size</definedName>
     <definedName name="CULC.cal_index_size" localSheetId="1">[3]!CULC.cal_index_size</definedName>
     <definedName name="CULC.cal_index_size">[3]!CULC.cal_index_size</definedName>
-    <definedName name="C保守単価" localSheetId="0">'[4]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守単価" localSheetId="2">'[4]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守単価" localSheetId="1">'[4]見積明細(ハードのみ）'!#REF!</definedName>
-    <definedName name="C保守単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守委託単価" localSheetId="0">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守委託単価" localSheetId="2">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守委託単価" localSheetId="1">'[4]見積明細(ハードのみ）'!#REF!</definedName>
@@ -110,6 +106,10 @@
     <definedName name="C保守支援単価" localSheetId="2">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守支援単価" localSheetId="1">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="C保守支援単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守単価" localSheetId="0">'[4]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守単価" localSheetId="2">'[4]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守単価" localSheetId="1">'[4]見積明細(ハードのみ）'!#REF!</definedName>
+    <definedName name="C保守単価">'[4]見積明細(ハードのみ）'!#REF!</definedName>
     <definedName name="DDDD" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="def" localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName name="def" localSheetId="2" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
@@ -361,90 +361,14 @@
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ" localSheetId="2">#REF!</definedName>
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ" localSheetId="1">#REF!</definedName>
     <definedName name="一般社員時間外労働手当部門別集計ｸｴﾘｰ">#REF!</definedName>
-    <definedName name="人日原価" localSheetId="0">#REF!</definedName>
-    <definedName name="人日原価" localSheetId="2">#REF!</definedName>
-    <definedName name="人日原価" localSheetId="1">#REF!</definedName>
-    <definedName name="人日原価">#REF!</definedName>
-    <definedName name="仕切り">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
-    <definedName name="仕切単価">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
-    <definedName name="住民税115" localSheetId="0">#REF!</definedName>
-    <definedName name="住民税115" localSheetId="2">#REF!</definedName>
-    <definedName name="住民税115" localSheetId="1">#REF!</definedName>
-    <definedName name="住民税115">#REF!</definedName>
-    <definedName name="住民税96" localSheetId="0">#REF!</definedName>
-    <definedName name="住民税96" localSheetId="2">#REF!</definedName>
-    <definedName name="住民税96" localSheetId="1">#REF!</definedName>
-    <definedName name="住民税96">#REF!</definedName>
-    <definedName name="住民税納付先の登録7" localSheetId="0">#REF!</definedName>
-    <definedName name="住民税納付先の登録7" localSheetId="2">#REF!</definedName>
-    <definedName name="住民税納付先の登録7" localSheetId="1">#REF!</definedName>
-    <definedName name="住民税納付先の登録7">#REF!</definedName>
+    <definedName name="印刷" localSheetId="0">[14]!印刷</definedName>
+    <definedName name="印刷" localSheetId="2">[14]!印刷</definedName>
+    <definedName name="印刷" localSheetId="1">[14]!印刷</definedName>
+    <definedName name="印刷">[14]!印刷</definedName>
     <definedName name="価格表" localSheetId="0">#REF!</definedName>
     <definedName name="価格表" localSheetId="2">#REF!</definedName>
     <definedName name="価格表" localSheetId="1">#REF!</definedName>
     <definedName name="価格表">#REF!</definedName>
-    <definedName name="保守単価">'[4]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
-    <definedName name="保守委託単価">'[4]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
-    <definedName name="保守支援単価">'[4]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
-    <definedName name="値引単価">'[4]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
-    <definedName name="備考">'[4]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
-    <definedName name="単価" localSheetId="0">#REF!</definedName>
-    <definedName name="単価" localSheetId="2">#REF!</definedName>
-    <definedName name="単価" localSheetId="1">#REF!</definedName>
-    <definedName name="単価">#REF!</definedName>
-    <definedName name="単価種別" localSheetId="0">#REF!</definedName>
-    <definedName name="単価種別" localSheetId="2">#REF!</definedName>
-    <definedName name="単価種別" localSheetId="1">#REF!</definedName>
-    <definedName name="単価種別">#REF!</definedName>
-    <definedName name="印刷" localSheetId="0">[14]!印刷</definedName>
-    <definedName name="印刷" localSheetId="2">[14]!印刷</definedName>
-    <definedName name="印刷" localSheetId="1">[14]!印刷</definedName>
-    <definedName name="印刷">[14]!印刷</definedName>
-    <definedName name="原価" localSheetId="0">#REF!</definedName>
-    <definedName name="原価" localSheetId="2">#REF!</definedName>
-    <definedName name="原価" localSheetId="1">#REF!</definedName>
-    <definedName name="原価">#REF!</definedName>
-    <definedName name="売値" localSheetId="0">#REF!</definedName>
-    <definedName name="売値" localSheetId="2">#REF!</definedName>
-    <definedName name="売値" localSheetId="1">#REF!</definedName>
-    <definedName name="売値">#REF!</definedName>
-    <definedName name="定価" localSheetId="0">#REF!</definedName>
-    <definedName name="定価" localSheetId="2">#REF!</definedName>
-    <definedName name="定価" localSheetId="1">#REF!</definedName>
-    <definedName name="定価">#REF!</definedName>
-    <definedName name="宿泊" localSheetId="0">#REF!</definedName>
-    <definedName name="宿泊" localSheetId="2">#REF!</definedName>
-    <definedName name="宿泊" localSheetId="1">#REF!</definedName>
-    <definedName name="宿泊">#REF!</definedName>
-    <definedName name="宿泊単金" localSheetId="0">#REF!</definedName>
-    <definedName name="宿泊単金" localSheetId="2">#REF!</definedName>
-    <definedName name="宿泊単金" localSheetId="1">#REF!</definedName>
-    <definedName name="宿泊単金">#REF!</definedName>
-    <definedName name="工程別生産性" localSheetId="0">#REF!</definedName>
-    <definedName name="工程別生産性" localSheetId="2">#REF!</definedName>
-    <definedName name="工程別生産性" localSheetId="1">#REF!</definedName>
-    <definedName name="工程別生産性">#REF!</definedName>
-    <definedName name="日帰り" localSheetId="0">#REF!</definedName>
-    <definedName name="日帰り" localSheetId="2">#REF!</definedName>
-    <definedName name="日帰り" localSheetId="1">#REF!</definedName>
-    <definedName name="日帰り">#REF!</definedName>
-    <definedName name="日帰り単金" localSheetId="0">#REF!</definedName>
-    <definedName name="日帰り単金" localSheetId="2">#REF!</definedName>
-    <definedName name="日帰り単金" localSheetId="1">#REF!</definedName>
-    <definedName name="日帰り単金">#REF!</definedName>
-    <definedName name="概要_基準日設定" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="概要_基準日設定" localSheetId="2" hidden="1">#REF!</definedName>
-    <definedName name="概要_基準日設定" localSheetId="1" hidden="1">#REF!</definedName>
-    <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
-    <definedName name="標準価格">'[4]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
-    <definedName name="機種SORT" localSheetId="0">[15]!機種SORT</definedName>
-    <definedName name="機種SORT" localSheetId="2">[15]!機種SORT</definedName>
-    <definedName name="機種SORT" localSheetId="1">[15]!機種SORT</definedName>
-    <definedName name="機種SORT">[16]!機種SORT</definedName>
-    <definedName name="機能別原価" localSheetId="0">#REF!</definedName>
-    <definedName name="機能別原価" localSheetId="2">#REF!</definedName>
-    <definedName name="機能別原価" localSheetId="1">#REF!</definedName>
-    <definedName name="機能別原価">#REF!</definedName>
     <definedName name="画面1" localSheetId="0">#REF!</definedName>
     <definedName name="画面1" localSheetId="2">#REF!</definedName>
     <definedName name="画面1" localSheetId="1">#REF!</definedName>
@@ -473,31 +397,23 @@
     <definedName name="画面7" localSheetId="2">#REF!</definedName>
     <definedName name="画面7" localSheetId="1">#REF!</definedName>
     <definedName name="画面7">#REF!</definedName>
-    <definedName name="直扱単価">'[4]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
-    <definedName name="社共単価">'[4]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
-    <definedName name="種別" localSheetId="0">#REF!</definedName>
-    <definedName name="種別" localSheetId="2">#REF!</definedName>
-    <definedName name="種別" localSheetId="1">#REF!</definedName>
-    <definedName name="種別">#REF!</definedName>
-    <definedName name="終了" localSheetId="0">[17]!終了</definedName>
-    <definedName name="終了" localSheetId="2">[17]!終了</definedName>
-    <definedName name="終了" localSheetId="1">[17]!終了</definedName>
-    <definedName name="終了">[17]!終了</definedName>
-    <definedName name="見やすく" localSheetId="0">[13]!見やすく</definedName>
-    <definedName name="見やすく" localSheetId="2">[13]!見やすく</definedName>
-    <definedName name="見やすく" localSheetId="1">[13]!見やすく</definedName>
-    <definedName name="見やすく">[13]!見やすく</definedName>
-    <definedName name="見積工数" localSheetId="0">#REF!</definedName>
-    <definedName name="見積工数" localSheetId="2">#REF!</definedName>
-    <definedName name="見積工数" localSheetId="1">#REF!</definedName>
-    <definedName name="見積工数">#REF!</definedName>
     <definedName name="解析">#N/A</definedName>
-    <definedName name="設計書">#N/A</definedName>
-    <definedName name="部">'[4]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
-    <definedName name="部門別時間外労働手当状況" localSheetId="0">#REF!</definedName>
-    <definedName name="部門別時間外労働手当状況" localSheetId="2">#REF!</definedName>
-    <definedName name="部門別時間外労働手当状況" localSheetId="1">#REF!</definedName>
-    <definedName name="部門別時間外労働手当状況">#REF!</definedName>
+    <definedName name="概要_基準日設定" localSheetId="0" hidden="1">#REF!</definedName>
+    <definedName name="概要_基準日設定" localSheetId="2" hidden="1">#REF!</definedName>
+    <definedName name="概要_基準日設定" localSheetId="1" hidden="1">#REF!</definedName>
+    <definedName name="概要_基準日設定" hidden="1">#REF!</definedName>
+    <definedName name="関連表" localSheetId="0" hidden="1">#REF!</definedName>
+    <definedName name="関連表" localSheetId="2" hidden="1">#REF!</definedName>
+    <definedName name="関連表" localSheetId="1" hidden="1">#REF!</definedName>
+    <definedName name="関連表" hidden="1">#REF!</definedName>
+    <definedName name="機種SORT" localSheetId="0">[15]!機種SORT</definedName>
+    <definedName name="機種SORT" localSheetId="2">[15]!機種SORT</definedName>
+    <definedName name="機種SORT" localSheetId="1">[15]!機種SORT</definedName>
+    <definedName name="機種SORT">[16]!機種SORT</definedName>
+    <definedName name="機能別原価" localSheetId="0">#REF!</definedName>
+    <definedName name="機能別原価" localSheetId="2">#REF!</definedName>
+    <definedName name="機能別原価" localSheetId="1">#REF!</definedName>
+    <definedName name="機能別原価">#REF!</definedName>
     <definedName name="銀行の登録48" localSheetId="0">#REF!</definedName>
     <definedName name="銀行の登録48" localSheetId="2">#REF!</definedName>
     <definedName name="銀行の登録48" localSheetId="1">#REF!</definedName>
@@ -510,14 +426,22 @@
     <definedName name="銀行の登録7" localSheetId="2">#REF!</definedName>
     <definedName name="銀行の登録7" localSheetId="1">#REF!</definedName>
     <definedName name="銀行の登録7">#REF!</definedName>
-    <definedName name="関連表" localSheetId="0" hidden="1">#REF!</definedName>
-    <definedName name="関連表" localSheetId="2" hidden="1">#REF!</definedName>
-    <definedName name="関連表" localSheetId="1" hidden="1">#REF!</definedName>
-    <definedName name="関連表" hidden="1">#REF!</definedName>
-    <definedName name="電車" localSheetId="0">#REF!</definedName>
-    <definedName name="電車" localSheetId="2">#REF!</definedName>
-    <definedName name="電車" localSheetId="1">#REF!</definedName>
-    <definedName name="電車">#REF!</definedName>
+    <definedName name="見やすく" localSheetId="0">[13]!見やすく</definedName>
+    <definedName name="見やすく" localSheetId="2">[13]!見やすく</definedName>
+    <definedName name="見やすく" localSheetId="1">[13]!見やすく</definedName>
+    <definedName name="見やすく">[13]!見やすく</definedName>
+    <definedName name="見積工数" localSheetId="0">#REF!</definedName>
+    <definedName name="見積工数" localSheetId="2">#REF!</definedName>
+    <definedName name="見積工数" localSheetId="1">#REF!</definedName>
+    <definedName name="見積工数">#REF!</definedName>
+    <definedName name="原価" localSheetId="0">#REF!</definedName>
+    <definedName name="原価" localSheetId="2">#REF!</definedName>
+    <definedName name="原価" localSheetId="1">#REF!</definedName>
+    <definedName name="原価">#REF!</definedName>
+    <definedName name="工程別生産性" localSheetId="0">#REF!</definedName>
+    <definedName name="工程別生産性" localSheetId="2">#REF!</definedName>
+    <definedName name="工程別生産性" localSheetId="1">#REF!</definedName>
+    <definedName name="工程別生産性">#REF!</definedName>
     <definedName name="項目名の登録1" localSheetId="0">#REF!</definedName>
     <definedName name="項目名の登録1" localSheetId="2">#REF!</definedName>
     <definedName name="項目名の登録1" localSheetId="1">#REF!</definedName>
@@ -550,10 +474,86 @@
     <definedName name="項目名の登録8" localSheetId="2">#REF!</definedName>
     <definedName name="項目名の登録8" localSheetId="1">#REF!</definedName>
     <definedName name="項目名の登録8">#REF!</definedName>
+    <definedName name="仕切り">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="仕切単価">'[4]見積明細(ハードのみ）'!$R$5:$R$34</definedName>
+    <definedName name="社共単価">'[4]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
+    <definedName name="種別" localSheetId="0">#REF!</definedName>
+    <definedName name="種別" localSheetId="2">#REF!</definedName>
+    <definedName name="種別" localSheetId="1">#REF!</definedName>
+    <definedName name="種別">#REF!</definedName>
+    <definedName name="終了" localSheetId="0">[17]!終了</definedName>
+    <definedName name="終了" localSheetId="2">[17]!終了</definedName>
+    <definedName name="終了" localSheetId="1">[17]!終了</definedName>
+    <definedName name="終了">[17]!終了</definedName>
+    <definedName name="住民税115" localSheetId="0">#REF!</definedName>
+    <definedName name="住民税115" localSheetId="2">#REF!</definedName>
+    <definedName name="住民税115" localSheetId="1">#REF!</definedName>
+    <definedName name="住民税115">#REF!</definedName>
+    <definedName name="住民税96" localSheetId="0">#REF!</definedName>
+    <definedName name="住民税96" localSheetId="2">#REF!</definedName>
+    <definedName name="住民税96" localSheetId="1">#REF!</definedName>
+    <definedName name="住民税96">#REF!</definedName>
+    <definedName name="住民税納付先の登録7" localSheetId="0">#REF!</definedName>
+    <definedName name="住民税納付先の登録7" localSheetId="2">#REF!</definedName>
+    <definedName name="住民税納付先の登録7" localSheetId="1">#REF!</definedName>
+    <definedName name="住民税納付先の登録7">#REF!</definedName>
+    <definedName name="宿泊" localSheetId="0">#REF!</definedName>
+    <definedName name="宿泊" localSheetId="2">#REF!</definedName>
+    <definedName name="宿泊" localSheetId="1">#REF!</definedName>
+    <definedName name="宿泊">#REF!</definedName>
+    <definedName name="宿泊単金" localSheetId="0">#REF!</definedName>
+    <definedName name="宿泊単金" localSheetId="2">#REF!</definedName>
+    <definedName name="宿泊単金" localSheetId="1">#REF!</definedName>
+    <definedName name="宿泊単金">#REF!</definedName>
+    <definedName name="人日原価" localSheetId="0">#REF!</definedName>
+    <definedName name="人日原価" localSheetId="2">#REF!</definedName>
+    <definedName name="人日原価" localSheetId="1">#REF!</definedName>
+    <definedName name="人日原価">#REF!</definedName>
+    <definedName name="設計書">#N/A</definedName>
+    <definedName name="単価" localSheetId="0">#REF!</definedName>
+    <definedName name="単価" localSheetId="2">#REF!</definedName>
+    <definedName name="単価" localSheetId="1">#REF!</definedName>
+    <definedName name="単価">#REF!</definedName>
+    <definedName name="単価種別" localSheetId="0">#REF!</definedName>
+    <definedName name="単価種別" localSheetId="2">#REF!</definedName>
+    <definedName name="単価種別" localSheetId="1">#REF!</definedName>
+    <definedName name="単価種別">#REF!</definedName>
+    <definedName name="値引単価">'[4]見積明細(ハードのみ）'!$J$5:$J$34</definedName>
+    <definedName name="直扱単価">'[4]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
+    <definedName name="定価" localSheetId="0">#REF!</definedName>
+    <definedName name="定価" localSheetId="2">#REF!</definedName>
+    <definedName name="定価" localSheetId="1">#REF!</definedName>
+    <definedName name="定価">#REF!</definedName>
+    <definedName name="電車" localSheetId="0">#REF!</definedName>
+    <definedName name="電車" localSheetId="2">#REF!</definedName>
+    <definedName name="電車" localSheetId="1">#REF!</definedName>
+    <definedName name="電車">#REF!</definedName>
+    <definedName name="日帰り" localSheetId="0">#REF!</definedName>
+    <definedName name="日帰り" localSheetId="2">#REF!</definedName>
+    <definedName name="日帰り" localSheetId="1">#REF!</definedName>
+    <definedName name="日帰り">#REF!</definedName>
+    <definedName name="日帰り単金" localSheetId="0">#REF!</definedName>
+    <definedName name="日帰り単金" localSheetId="2">#REF!</definedName>
+    <definedName name="日帰り単金" localSheetId="1">#REF!</definedName>
+    <definedName name="日帰り単金">#REF!</definedName>
+    <definedName name="売値" localSheetId="0">#REF!</definedName>
+    <definedName name="売値" localSheetId="2">#REF!</definedName>
+    <definedName name="売値" localSheetId="1">#REF!</definedName>
+    <definedName name="売値">#REF!</definedName>
     <definedName name="飛行機" localSheetId="0">#REF!</definedName>
     <definedName name="飛行機" localSheetId="2">#REF!</definedName>
     <definedName name="飛行機" localSheetId="1">#REF!</definedName>
     <definedName name="飛行機">#REF!</definedName>
+    <definedName name="備考">'[4]見積明細(ハードのみ）'!$AA$5:$AA$34</definedName>
+    <definedName name="標準価格">'[4]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
+    <definedName name="部">'[4]見積明細(ハードのみ）'!$Z$5:$Z$34</definedName>
+    <definedName name="部門別時間外労働手当状況" localSheetId="0">#REF!</definedName>
+    <definedName name="部門別時間外労働手当状況" localSheetId="2">#REF!</definedName>
+    <definedName name="部門別時間外労働手当状況" localSheetId="1">#REF!</definedName>
+    <definedName name="部門別時間外労働手当状況">#REF!</definedName>
+    <definedName name="保守委託単価">'[4]見積明細(ハードのみ）'!$N$5:$N$34</definedName>
+    <definedName name="保守支援単価">'[4]見積明細(ハードのみ）'!$P$5:$P$34</definedName>
+    <definedName name="保守単価">'[4]見積明細(ハードのみ）'!$L$5:$L$34</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -569,20 +569,6 @@
     <phoneticPr fontId="11"/>
   </si>
   <si>
-    <t>フェーズ2⇒</t>
-    <phoneticPr fontId="11"/>
-  </si>
-  <si>
-    <t>フェーズ3⇒</t>
-  </si>
-  <si>
-    <t>フェーズ4⇒</t>
-  </si>
-  <si>
-    <t>フェーズ1⇒</t>
-    <phoneticPr fontId="11"/>
-  </si>
-  <si>
     <t>申請名</t>
     <rPh sb="0" eb="2">
       <t>シンセイ</t>
@@ -593,8 +579,19 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>フェーズ5</t>
-    <phoneticPr fontId="5"/>
+    <t>レベル1</t>
+  </si>
+  <si>
+    <t>←レベル2</t>
+  </si>
+  <si>
+    <t>←レベル3</t>
+  </si>
+  <si>
+    <t>←レベル4</t>
+  </si>
+  <si>
+    <t>←レベル5</t>
   </si>
 </sst>
 </file>
@@ -896,9 +893,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
+      <sheetName val="master"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -911,7 +910,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -922,6 +921,7 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="項目定義書"/>
+      <sheetName val="テーブル設計991127"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1">
@@ -3412,7 +3412,7 @@
             <v>1</v>
           </cell>
           <cell r="E170" t="str">
-            <v>'0':未処理、'1':仮処理、'2':本処理、'3':出力不要</v>
+            <v xml:space="preserve">'0':未処理、'1':仮処理、'2':本処理、'3':出力不要 </v>
           </cell>
         </row>
         <row r="171">
@@ -6202,6 +6202,7 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6224,17 +6225,17 @@
       <sheetName val="内示書"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6571,6 +6572,8 @@
       <sheetName val="見積明細(ハード三菱分のみ）"/>
       <sheetName val="見積明細(PP料含む） (2)"/>
       <sheetName val="費用比較 "/>
+      <sheetName val="ﾊｰﾄﾞ明細(FT1200）"/>
+      <sheetName val="master"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1">
@@ -6621,8 +6624,8 @@
           <cell r="Z5" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA5" t="str">
-            <v/>
+          <cell r="AA5">
+            <v>0</v>
           </cell>
         </row>
         <row r="6">
@@ -6671,8 +6674,8 @@
           <cell r="Z6" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA6" t="str">
-            <v/>
+          <cell r="AA6">
+            <v>0</v>
           </cell>
         </row>
         <row r="7">
@@ -6774,8 +6777,8 @@
           <cell r="Z8" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA8" t="str">
-            <v/>
+          <cell r="AA8">
+            <v>0</v>
           </cell>
         </row>
         <row r="9">
@@ -6826,8 +6829,8 @@
           <cell r="Z9" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA9" t="str">
-            <v/>
+          <cell r="AA9">
+            <v>0</v>
           </cell>
         </row>
         <row r="10">
@@ -6877,8 +6880,8 @@
           <cell r="Z10" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA10" t="str">
-            <v/>
+          <cell r="AA10">
+            <v>0</v>
           </cell>
         </row>
         <row r="11">
@@ -6929,8 +6932,8 @@
           <cell r="Z11" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA11" t="str">
-            <v/>
+          <cell r="AA11">
+            <v>0</v>
           </cell>
         </row>
         <row r="12">
@@ -6980,8 +6983,8 @@
           <cell r="Z12" t="str">
             <v>AC</v>
           </cell>
-          <cell r="AA12" t="str">
-            <v/>
+          <cell r="AA12">
+            <v>0</v>
           </cell>
         </row>
         <row r="13">
@@ -7084,8 +7087,8 @@
           <cell r="Z14" t="str">
             <v>MC</v>
           </cell>
-          <cell r="AA14" t="str">
-            <v/>
+          <cell r="AA14">
+            <v>0</v>
           </cell>
         </row>
         <row r="15">
@@ -7135,8 +7138,8 @@
           <cell r="Z15" t="str">
             <v>MC</v>
           </cell>
-          <cell r="AA15" t="str">
-            <v/>
+          <cell r="AA15">
+            <v>0</v>
           </cell>
         </row>
         <row r="16">
@@ -7161,11 +7164,11 @@
           <cell r="L16">
             <v>60000</v>
           </cell>
-          <cell r="N16" t="str">
-            <v/>
-          </cell>
-          <cell r="P16" t="str">
-            <v/>
+          <cell r="N16">
+            <v>0</v>
+          </cell>
+          <cell r="P16">
+            <v>0</v>
           </cell>
           <cell r="R16">
             <v>421200</v>
@@ -7179,16 +7182,16 @@
           <cell r="X16">
             <v>0</v>
           </cell>
-          <cell r="Z16" t="str">
-            <v/>
-          </cell>
-          <cell r="AA16" t="str">
-            <v/>
+          <cell r="Z16">
+            <v>0</v>
+          </cell>
+          <cell r="AA16">
+            <v>0</v>
           </cell>
         </row>
         <row r="17">
-          <cell r="D17" t="str">
-            <v/>
+          <cell r="D17">
+            <v>0</v>
           </cell>
           <cell r="E17" t="str">
             <v>ﾌﾟﾘﾝﾀｹｰﾌﾞﾙ</v>
@@ -7208,11 +7211,11 @@
           <cell r="L17">
             <v>0</v>
           </cell>
-          <cell r="N17" t="str">
-            <v/>
-          </cell>
-          <cell r="P17" t="str">
-            <v/>
+          <cell r="N17">
+            <v>0</v>
+          </cell>
+          <cell r="P17">
+            <v>0</v>
           </cell>
           <cell r="R17">
             <v>1300</v>
@@ -7226,22 +7229,22 @@
           <cell r="X17">
             <v>0</v>
           </cell>
-          <cell r="Z17" t="str">
-            <v/>
-          </cell>
-          <cell r="AA17" t="str">
-            <v/>
+          <cell r="Z17">
+            <v>0</v>
+          </cell>
+          <cell r="AA17">
+            <v>0</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="D18" t="str">
-            <v/>
+          <cell r="D18">
+            <v>0</v>
           </cell>
           <cell r="E18" t="str">
             <v>ハンディターミナル  ＢＨＴ－６０００（１ＭＢ）</v>
           </cell>
-          <cell r="F18" t="str">
-            <v/>
+          <cell r="F18">
+            <v>0</v>
           </cell>
           <cell r="G18">
             <v>6</v>
@@ -7255,11 +7258,11 @@
           <cell r="L18">
             <v>0</v>
           </cell>
-          <cell r="N18" t="str">
-            <v/>
-          </cell>
-          <cell r="P18" t="str">
-            <v/>
+          <cell r="N18">
+            <v>0</v>
+          </cell>
+          <cell r="P18">
+            <v>0</v>
           </cell>
           <cell r="R18">
             <v>138600</v>
@@ -7273,22 +7276,22 @@
           <cell r="X18">
             <v>0</v>
           </cell>
-          <cell r="Z18" t="str">
-            <v/>
-          </cell>
-          <cell r="AA18" t="str">
-            <v/>
+          <cell r="Z18">
+            <v>0</v>
+          </cell>
+          <cell r="AA18">
+            <v>0</v>
           </cell>
         </row>
         <row r="19">
-          <cell r="D19" t="str">
-            <v/>
+          <cell r="D19">
+            <v>0</v>
           </cell>
           <cell r="E19" t="str">
             <v>光通信ユニット</v>
           </cell>
-          <cell r="F19" t="str">
-            <v/>
+          <cell r="F19">
+            <v>0</v>
           </cell>
           <cell r="G19">
             <v>2</v>
@@ -7302,11 +7305,11 @@
           <cell r="L19">
             <v>0</v>
           </cell>
-          <cell r="N19" t="str">
-            <v/>
-          </cell>
-          <cell r="P19" t="str">
-            <v/>
+          <cell r="N19">
+            <v>0</v>
+          </cell>
+          <cell r="P19">
+            <v>0</v>
           </cell>
           <cell r="R19">
             <v>46000</v>
@@ -7320,22 +7323,22 @@
           <cell r="X19">
             <v>0</v>
           </cell>
-          <cell r="Z19" t="str">
-            <v/>
-          </cell>
-          <cell r="AA19" t="str">
-            <v/>
+          <cell r="Z19">
+            <v>0</v>
+          </cell>
+          <cell r="AA19">
+            <v>0</v>
           </cell>
         </row>
         <row r="20">
-          <cell r="D20" t="str">
-            <v/>
+          <cell r="D20">
+            <v>0</v>
           </cell>
           <cell r="E20" t="str">
             <v>ＮｉＭＨバッテリーパック</v>
           </cell>
-          <cell r="F20" t="str">
-            <v/>
+          <cell r="F20">
+            <v>0</v>
           </cell>
           <cell r="G20">
             <v>6</v>
@@ -7349,11 +7352,11 @@
           <cell r="L20">
             <v>0</v>
           </cell>
-          <cell r="N20" t="str">
-            <v/>
-          </cell>
-          <cell r="P20" t="str">
-            <v/>
+          <cell r="N20">
+            <v>0</v>
+          </cell>
+          <cell r="P20">
+            <v>0</v>
           </cell>
           <cell r="R20">
             <v>6000</v>
@@ -7367,22 +7370,22 @@
           <cell r="X20">
             <v>0</v>
           </cell>
-          <cell r="Z20" t="str">
-            <v/>
-          </cell>
-          <cell r="AA20" t="str">
-            <v/>
+          <cell r="Z20">
+            <v>0</v>
+          </cell>
+          <cell r="AA20">
+            <v>0</v>
           </cell>
         </row>
         <row r="21">
-          <cell r="D21" t="str">
-            <v/>
+          <cell r="D21">
+            <v>0</v>
           </cell>
           <cell r="E21" t="str">
             <v>ＲＳ２３２Ｃケーブル</v>
           </cell>
-          <cell r="F21" t="str">
-            <v/>
+          <cell r="F21">
+            <v>0</v>
           </cell>
           <cell r="G21">
             <v>2</v>
@@ -7396,11 +7399,11 @@
           <cell r="L21">
             <v>0</v>
           </cell>
-          <cell r="N21" t="str">
-            <v/>
-          </cell>
-          <cell r="P21" t="str">
-            <v/>
+          <cell r="N21">
+            <v>0</v>
+          </cell>
+          <cell r="P21">
+            <v>0</v>
           </cell>
           <cell r="R21">
             <v>9000</v>
@@ -7414,22 +7417,22 @@
           <cell r="X21">
             <v>0</v>
           </cell>
-          <cell r="Z21" t="str">
-            <v/>
-          </cell>
-          <cell r="AA21" t="str">
-            <v/>
+          <cell r="Z21">
+            <v>0</v>
+          </cell>
+          <cell r="AA21">
+            <v>0</v>
           </cell>
         </row>
         <row r="22">
-          <cell r="D22" t="str">
-            <v/>
+          <cell r="D22">
+            <v>0</v>
           </cell>
           <cell r="E22" t="str">
             <v>ＣＵ転送ユーティリティ</v>
           </cell>
-          <cell r="F22" t="str">
-            <v/>
+          <cell r="F22">
+            <v>0</v>
           </cell>
           <cell r="G22">
             <v>1</v>
@@ -7443,11 +7446,11 @@
           <cell r="L22">
             <v>0</v>
           </cell>
-          <cell r="N22" t="str">
-            <v/>
-          </cell>
-          <cell r="P22" t="str">
-            <v/>
+          <cell r="N22">
+            <v>0</v>
+          </cell>
+          <cell r="P22">
+            <v>0</v>
           </cell>
           <cell r="R22">
             <v>35000</v>
@@ -7461,22 +7464,22 @@
           <cell r="X22">
             <v>0</v>
           </cell>
-          <cell r="Z22" t="str">
-            <v/>
-          </cell>
-          <cell r="AA22" t="str">
-            <v/>
+          <cell r="Z22">
+            <v>0</v>
+          </cell>
+          <cell r="AA22">
+            <v>0</v>
           </cell>
         </row>
         <row r="23">
-          <cell r="D23" t="str">
-            <v/>
+          <cell r="D23">
+            <v>0</v>
           </cell>
           <cell r="E23" t="str">
             <v>ＢＨＴ－ＢＡＳＩＣ３，１</v>
           </cell>
-          <cell r="F23" t="str">
-            <v/>
+          <cell r="F23">
+            <v>0</v>
           </cell>
           <cell r="G23">
             <v>1</v>
@@ -7490,11 +7493,11 @@
           <cell r="L23">
             <v>0</v>
           </cell>
-          <cell r="N23" t="str">
-            <v/>
-          </cell>
-          <cell r="P23" t="str">
-            <v/>
+          <cell r="N23">
+            <v>0</v>
+          </cell>
+          <cell r="P23">
+            <v>0</v>
           </cell>
           <cell r="R23">
             <v>32000</v>
@@ -7508,22 +7511,22 @@
           <cell r="X23">
             <v>0</v>
           </cell>
-          <cell r="Z23" t="str">
-            <v/>
-          </cell>
-          <cell r="AA23" t="str">
-            <v/>
+          <cell r="Z23">
+            <v>0</v>
+          </cell>
+          <cell r="AA23">
+            <v>0</v>
           </cell>
         </row>
         <row r="24">
-          <cell r="D24" t="str">
-            <v/>
+          <cell r="D24">
+            <v>0</v>
           </cell>
           <cell r="E24" t="str">
             <v>ＨＵＢ</v>
           </cell>
-          <cell r="F24" t="str">
-            <v/>
+          <cell r="F24">
+            <v>0</v>
           </cell>
           <cell r="G24">
             <v>3</v>
@@ -7537,11 +7540,11 @@
           <cell r="L24">
             <v>0</v>
           </cell>
-          <cell r="N24" t="str">
-            <v/>
-          </cell>
-          <cell r="P24" t="str">
-            <v/>
+          <cell r="N24">
+            <v>0</v>
+          </cell>
+          <cell r="P24">
+            <v>0</v>
           </cell>
           <cell r="R24">
             <v>11000</v>
@@ -7555,22 +7558,22 @@
           <cell r="X24">
             <v>0</v>
           </cell>
-          <cell r="Z24" t="str">
-            <v/>
-          </cell>
-          <cell r="AA24" t="str">
-            <v/>
+          <cell r="Z24">
+            <v>0</v>
+          </cell>
+          <cell r="AA24">
+            <v>0</v>
           </cell>
         </row>
         <row r="25">
-          <cell r="D25" t="str">
-            <v/>
+          <cell r="D25">
+            <v>0</v>
           </cell>
           <cell r="E25" t="str">
             <v>10BASE-Tｹｰﾌﾞﾙ</v>
           </cell>
-          <cell r="F25" t="str">
-            <v/>
+          <cell r="F25">
+            <v>0</v>
           </cell>
           <cell r="G25">
             <v>10</v>
@@ -7584,11 +7587,11 @@
           <cell r="L25">
             <v>0</v>
           </cell>
-          <cell r="N25" t="str">
-            <v/>
-          </cell>
-          <cell r="P25" t="str">
-            <v/>
+          <cell r="N25">
+            <v>0</v>
+          </cell>
+          <cell r="P25">
+            <v>0</v>
           </cell>
           <cell r="R25">
             <v>3200</v>
@@ -7602,22 +7605,22 @@
           <cell r="X25">
             <v>0</v>
           </cell>
-          <cell r="Z25" t="str">
-            <v/>
-          </cell>
-          <cell r="AA25" t="str">
-            <v/>
+          <cell r="Z25">
+            <v>0</v>
+          </cell>
+          <cell r="AA25">
+            <v>0</v>
           </cell>
         </row>
         <row r="26">
-          <cell r="D26" t="str">
-            <v/>
+          <cell r="D26">
+            <v>0</v>
           </cell>
           <cell r="E26" t="str">
             <v>Microsoft Office97</v>
           </cell>
-          <cell r="F26" t="str">
-            <v/>
+          <cell r="F26">
+            <v>0</v>
           </cell>
           <cell r="G26">
             <v>1</v>
@@ -7631,11 +7634,11 @@
           <cell r="L26">
             <v>0</v>
           </cell>
-          <cell r="N26" t="str">
-            <v/>
-          </cell>
-          <cell r="P26" t="str">
-            <v/>
+          <cell r="N26">
+            <v>0</v>
+          </cell>
+          <cell r="P26">
+            <v>0</v>
           </cell>
           <cell r="R26">
             <v>55000</v>
@@ -7649,22 +7652,22 @@
           <cell r="X26">
             <v>0</v>
           </cell>
-          <cell r="Z26" t="str">
-            <v/>
-          </cell>
-          <cell r="AA26" t="str">
-            <v/>
+          <cell r="Z26">
+            <v>0</v>
+          </cell>
+          <cell r="AA26">
+            <v>0</v>
           </cell>
         </row>
         <row r="27">
-          <cell r="D27" t="str">
-            <v/>
+          <cell r="D27">
+            <v>0</v>
           </cell>
           <cell r="E27" t="str">
             <v>DATE NATURE２</v>
           </cell>
-          <cell r="F27" t="str">
-            <v/>
+          <cell r="F27">
+            <v>0</v>
           </cell>
           <cell r="G27">
             <v>2</v>
@@ -7678,11 +7681,11 @@
           <cell r="L27">
             <v>0</v>
           </cell>
-          <cell r="N27" t="str">
-            <v/>
-          </cell>
-          <cell r="P27" t="str">
-            <v/>
+          <cell r="N27">
+            <v>0</v>
+          </cell>
+          <cell r="P27">
+            <v>0</v>
           </cell>
           <cell r="R27">
             <v>39800</v>
@@ -7696,43 +7699,43 @@
           <cell r="X27">
             <v>0</v>
           </cell>
-          <cell r="Z27" t="str">
-            <v/>
-          </cell>
-          <cell r="AA27" t="str">
-            <v/>
+          <cell r="Z27">
+            <v>0</v>
+          </cell>
+          <cell r="AA27">
+            <v>0</v>
           </cell>
         </row>
         <row r="28">
-          <cell r="D28" t="str">
-            <v/>
-          </cell>
-          <cell r="E28" t="str">
-            <v/>
-          </cell>
-          <cell r="F28" t="str">
-            <v/>
-          </cell>
-          <cell r="G28" t="str">
-            <v/>
-          </cell>
-          <cell r="H28" t="str">
-            <v/>
+          <cell r="D28">
+            <v>0</v>
+          </cell>
+          <cell r="E28">
+            <v>0</v>
+          </cell>
+          <cell r="F28">
+            <v>0</v>
+          </cell>
+          <cell r="G28">
+            <v>0</v>
+          </cell>
+          <cell r="H28">
+            <v>0</v>
           </cell>
           <cell r="J28">
             <v>0</v>
           </cell>
-          <cell r="L28" t="str">
-            <v/>
-          </cell>
-          <cell r="N28" t="str">
-            <v/>
-          </cell>
-          <cell r="P28" t="str">
-            <v/>
-          </cell>
-          <cell r="R28" t="str">
-            <v/>
+          <cell r="L28">
+            <v>0</v>
+          </cell>
+          <cell r="N28">
+            <v>0</v>
+          </cell>
+          <cell r="P28">
+            <v>0</v>
+          </cell>
+          <cell r="R28">
+            <v>0</v>
           </cell>
           <cell r="T28">
             <v>0</v>
@@ -7743,43 +7746,43 @@
           <cell r="X28">
             <v>0</v>
           </cell>
-          <cell r="Z28" t="str">
-            <v/>
-          </cell>
-          <cell r="AA28" t="str">
-            <v/>
+          <cell r="Z28">
+            <v>0</v>
+          </cell>
+          <cell r="AA28">
+            <v>0</v>
           </cell>
         </row>
         <row r="29">
-          <cell r="D29" t="str">
-            <v/>
-          </cell>
-          <cell r="E29" t="str">
-            <v/>
-          </cell>
-          <cell r="F29" t="str">
-            <v/>
-          </cell>
-          <cell r="G29" t="str">
-            <v/>
-          </cell>
-          <cell r="H29" t="str">
-            <v/>
+          <cell r="D29">
+            <v>0</v>
+          </cell>
+          <cell r="E29">
+            <v>0</v>
+          </cell>
+          <cell r="F29">
+            <v>0</v>
+          </cell>
+          <cell r="G29">
+            <v>0</v>
+          </cell>
+          <cell r="H29">
+            <v>0</v>
           </cell>
           <cell r="J29">
             <v>0</v>
           </cell>
-          <cell r="L29" t="str">
-            <v/>
-          </cell>
-          <cell r="N29" t="str">
-            <v/>
-          </cell>
-          <cell r="P29" t="str">
-            <v/>
-          </cell>
-          <cell r="R29" t="str">
-            <v/>
+          <cell r="L29">
+            <v>0</v>
+          </cell>
+          <cell r="N29">
+            <v>0</v>
+          </cell>
+          <cell r="P29">
+            <v>0</v>
+          </cell>
+          <cell r="R29">
+            <v>0</v>
           </cell>
           <cell r="T29">
             <v>0</v>
@@ -7790,43 +7793,43 @@
           <cell r="X29">
             <v>0</v>
           </cell>
-          <cell r="Z29" t="str">
-            <v/>
-          </cell>
-          <cell r="AA29" t="str">
-            <v/>
+          <cell r="Z29">
+            <v>0</v>
+          </cell>
+          <cell r="AA29">
+            <v>0</v>
           </cell>
         </row>
         <row r="30">
-          <cell r="D30" t="str">
-            <v/>
-          </cell>
-          <cell r="E30" t="str">
-            <v/>
-          </cell>
-          <cell r="F30" t="str">
-            <v/>
-          </cell>
-          <cell r="G30" t="str">
-            <v/>
-          </cell>
-          <cell r="H30" t="str">
-            <v/>
+          <cell r="D30">
+            <v>0</v>
+          </cell>
+          <cell r="E30">
+            <v>0</v>
+          </cell>
+          <cell r="F30">
+            <v>0</v>
+          </cell>
+          <cell r="G30">
+            <v>0</v>
+          </cell>
+          <cell r="H30">
+            <v>0</v>
           </cell>
           <cell r="J30">
             <v>0</v>
           </cell>
-          <cell r="L30" t="str">
-            <v/>
-          </cell>
-          <cell r="N30" t="str">
-            <v/>
-          </cell>
-          <cell r="P30" t="str">
-            <v/>
-          </cell>
-          <cell r="R30" t="str">
-            <v/>
+          <cell r="L30">
+            <v>0</v>
+          </cell>
+          <cell r="N30">
+            <v>0</v>
+          </cell>
+          <cell r="P30">
+            <v>0</v>
+          </cell>
+          <cell r="R30">
+            <v>0</v>
           </cell>
           <cell r="T30">
             <v>0</v>
@@ -7837,43 +7840,43 @@
           <cell r="X30">
             <v>0</v>
           </cell>
-          <cell r="Z30" t="str">
-            <v/>
-          </cell>
-          <cell r="AA30" t="str">
-            <v/>
+          <cell r="Z30">
+            <v>0</v>
+          </cell>
+          <cell r="AA30">
+            <v>0</v>
           </cell>
         </row>
         <row r="31">
-          <cell r="D31" t="str">
-            <v/>
-          </cell>
-          <cell r="E31" t="str">
-            <v/>
-          </cell>
-          <cell r="F31" t="str">
-            <v/>
-          </cell>
-          <cell r="G31" t="str">
-            <v/>
-          </cell>
-          <cell r="H31" t="str">
-            <v/>
+          <cell r="D31">
+            <v>0</v>
+          </cell>
+          <cell r="E31">
+            <v>0</v>
+          </cell>
+          <cell r="F31">
+            <v>0</v>
+          </cell>
+          <cell r="G31">
+            <v>0</v>
+          </cell>
+          <cell r="H31">
+            <v>0</v>
           </cell>
           <cell r="J31">
             <v>0</v>
           </cell>
-          <cell r="L31" t="str">
-            <v/>
-          </cell>
-          <cell r="N31" t="str">
-            <v/>
-          </cell>
-          <cell r="P31" t="str">
-            <v/>
-          </cell>
-          <cell r="R31" t="str">
-            <v/>
+          <cell r="L31">
+            <v>0</v>
+          </cell>
+          <cell r="N31">
+            <v>0</v>
+          </cell>
+          <cell r="P31">
+            <v>0</v>
+          </cell>
+          <cell r="R31">
+            <v>0</v>
           </cell>
           <cell r="T31">
             <v>0</v>
@@ -7884,43 +7887,43 @@
           <cell r="X31">
             <v>0</v>
           </cell>
-          <cell r="Z31" t="str">
-            <v/>
-          </cell>
-          <cell r="AA31" t="str">
-            <v/>
+          <cell r="Z31">
+            <v>0</v>
+          </cell>
+          <cell r="AA31">
+            <v>0</v>
           </cell>
         </row>
         <row r="32">
-          <cell r="D32" t="str">
-            <v/>
-          </cell>
-          <cell r="E32" t="str">
-            <v/>
-          </cell>
-          <cell r="F32" t="str">
-            <v/>
-          </cell>
-          <cell r="G32" t="str">
-            <v/>
-          </cell>
-          <cell r="H32" t="str">
-            <v/>
+          <cell r="D32">
+            <v>0</v>
+          </cell>
+          <cell r="E32">
+            <v>0</v>
+          </cell>
+          <cell r="F32">
+            <v>0</v>
+          </cell>
+          <cell r="G32">
+            <v>0</v>
+          </cell>
+          <cell r="H32">
+            <v>0</v>
           </cell>
           <cell r="J32">
             <v>0</v>
           </cell>
-          <cell r="L32" t="str">
-            <v/>
-          </cell>
-          <cell r="N32" t="str">
-            <v/>
-          </cell>
-          <cell r="P32" t="str">
-            <v/>
-          </cell>
-          <cell r="R32" t="str">
-            <v/>
+          <cell r="L32">
+            <v>0</v>
+          </cell>
+          <cell r="N32">
+            <v>0</v>
+          </cell>
+          <cell r="P32">
+            <v>0</v>
+          </cell>
+          <cell r="R32">
+            <v>0</v>
           </cell>
           <cell r="T32">
             <v>0</v>
@@ -7931,43 +7934,43 @@
           <cell r="X32">
             <v>0</v>
           </cell>
-          <cell r="Z32" t="str">
-            <v/>
-          </cell>
-          <cell r="AA32" t="str">
-            <v/>
+          <cell r="Z32">
+            <v>0</v>
+          </cell>
+          <cell r="AA32">
+            <v>0</v>
           </cell>
         </row>
         <row r="33">
-          <cell r="D33" t="str">
-            <v/>
-          </cell>
-          <cell r="E33" t="str">
-            <v/>
-          </cell>
-          <cell r="F33" t="str">
-            <v/>
-          </cell>
-          <cell r="G33" t="str">
-            <v/>
-          </cell>
-          <cell r="H33" t="str">
-            <v/>
+          <cell r="D33">
+            <v>0</v>
+          </cell>
+          <cell r="E33">
+            <v>0</v>
+          </cell>
+          <cell r="F33">
+            <v>0</v>
+          </cell>
+          <cell r="G33">
+            <v>0</v>
+          </cell>
+          <cell r="H33">
+            <v>0</v>
           </cell>
           <cell r="J33">
             <v>0</v>
           </cell>
-          <cell r="L33" t="str">
-            <v/>
-          </cell>
-          <cell r="N33" t="str">
-            <v/>
-          </cell>
-          <cell r="P33" t="str">
-            <v/>
-          </cell>
-          <cell r="R33" t="str">
-            <v/>
+          <cell r="L33">
+            <v>0</v>
+          </cell>
+          <cell r="N33">
+            <v>0</v>
+          </cell>
+          <cell r="P33">
+            <v>0</v>
+          </cell>
+          <cell r="R33">
+            <v>0</v>
           </cell>
           <cell r="T33">
             <v>0</v>
@@ -7978,43 +7981,43 @@
           <cell r="X33">
             <v>0</v>
           </cell>
-          <cell r="Z33" t="str">
-            <v/>
-          </cell>
-          <cell r="AA33" t="str">
-            <v/>
+          <cell r="Z33">
+            <v>0</v>
+          </cell>
+          <cell r="AA33">
+            <v>0</v>
           </cell>
         </row>
         <row r="34">
-          <cell r="D34" t="str">
-            <v/>
-          </cell>
-          <cell r="E34" t="str">
-            <v/>
-          </cell>
-          <cell r="F34" t="str">
-            <v/>
-          </cell>
-          <cell r="G34" t="str">
-            <v/>
-          </cell>
-          <cell r="H34" t="str">
-            <v/>
+          <cell r="D34">
+            <v>0</v>
+          </cell>
+          <cell r="E34">
+            <v>0</v>
+          </cell>
+          <cell r="F34">
+            <v>0</v>
+          </cell>
+          <cell r="G34">
+            <v>0</v>
+          </cell>
+          <cell r="H34">
+            <v>0</v>
           </cell>
           <cell r="J34">
             <v>0</v>
           </cell>
-          <cell r="L34" t="str">
-            <v/>
-          </cell>
-          <cell r="N34" t="str">
-            <v/>
-          </cell>
-          <cell r="P34" t="str">
-            <v/>
-          </cell>
-          <cell r="R34" t="str">
-            <v/>
+          <cell r="L34">
+            <v>0</v>
+          </cell>
+          <cell r="N34">
+            <v>0</v>
+          </cell>
+          <cell r="P34">
+            <v>0</v>
+          </cell>
+          <cell r="R34">
+            <v>0</v>
           </cell>
           <cell r="T34">
             <v>0</v>
@@ -8025,18 +8028,20 @@
           <cell r="X34">
             <v>0</v>
           </cell>
-          <cell r="Z34" t="str">
-            <v/>
-          </cell>
-          <cell r="AA34" t="str">
-            <v/>
+          <cell r="Z34">
+            <v>0</v>
+          </cell>
+          <cell r="AA34">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8047,6 +8052,7 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="仕切価格"/>
+      <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1">
@@ -8225,7 +8231,7 @@
             <v>型番</v>
           </cell>
           <cell r="D2" t="str">
-            <v>製品名</v>
+            <v xml:space="preserve">製品名 </v>
           </cell>
           <cell r="E2" t="str">
             <v>仕様</v>
@@ -29806,7 +29812,7 @@
             <v>ACW-CD-S</v>
           </cell>
           <cell r="C140" t="str">
-            <v>M6754-5</v>
+            <v xml:space="preserve">M6754-5 </v>
           </cell>
           <cell r="D140" t="str">
             <v>内蔵CD-ROM装置</v>
@@ -44397,6 +44403,7 @@
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -44409,7 +44416,7 @@
       <sheetName val="１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -44755,8 +44762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="55" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B40"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12"/>
@@ -44809,25 +44816,25 @@
     <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="3"/>
       <c r="B3" s="7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="8" t="s">
@@ -44857,8 +44864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A2" zoomScale="160" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12"/>
@@ -44911,25 +44918,25 @@
     <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="3"/>
       <c r="B3" s="7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="8" t="s">
@@ -44959,8 +44966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScale="55" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="12"/>
@@ -45013,25 +45020,25 @@
     <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="3"/>
       <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="8" t="s">

</xml_diff>